<commit_message>
update user story, update document, update file query
</commit_message>
<xml_diff>
--- a/UML/use_case.xlsx
+++ b/UML/use_case.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Nam 3\NMCNPM\DoAn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\University\Subject\NMCNPM\DoAn\project\QuanLyHoiNghi\UML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EA064C-CA5A-4962-966F-AFD6CC74CD5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -303,7 +302,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -419,7 +418,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,7 +434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,23 +509,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -562,23 +544,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -754,11 +719,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1503,7 +1468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1515,7 +1480,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>